<commit_message>
Finishing the model and clearing out the port model files
</commit_message>
<xml_diff>
--- a/Copy of literatur review.xlsx
+++ b/Copy of literatur review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vegar\Desktop\Pricing climate risk in shipping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DD0E9D-AAAD-4FC5-B508-B4E6340D36EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E351F25-2F69-4238-A1D0-FB088076EE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{812CBD80-D656-4644-AAE1-2F9B4CE08848}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{812CBD80-D656-4644-AAE1-2F9B4CE08848}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="268">
   <si>
     <t>link</t>
   </si>
@@ -635,12 +635,323 @@
 - Find arrival rate and service rate for Tin Can Island Port. 
 - Argue that the exisiting capacity is sufficient but they identify why congestion happens</t>
   </si>
+  <si>
+    <t>Syriopoulos et.al 2023</t>
+  </si>
+  <si>
+    <t>Hedging Strategies in Carbon Emission Price Dynamics: Implications for Shipping Markets</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/1996-1073/16/17/6396</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Investigates the different hedging strategies to headge carbon risk in shipping, in particular bunker fuel risk.
+- Investigates OLS, Error Correction Model (ECM), Asymmetric Dynamic Conditional Correlation (ADCC) Model and  Student’s t-Copula (t-Copula) Models.
+- Carbon futures is an effective hedge for carbon price, simple models work well, Brent futures dominates other petrolium contracts for headging effectiveness, carbon spot-future is a very effective hedging strategy, 
+</t>
+  </si>
+  <si>
+    <t>Gritsenko 2017</t>
+  </si>
+  <si>
+    <t>Regulating GHG Emissions from shipping: Local, global, or polycentric approach?</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0308597X17301215?via%3Dihub</t>
+  </si>
+  <si>
+    <t>This paper examines the recent literature on polycentric climate governance and suggests principles for environmental regulation in shipping based on a polycentric approach.</t>
+  </si>
+  <si>
+    <t>Hermeling et.al 2015</t>
+  </si>
+  <si>
+    <t>Sailing into a dilemma: An economic and legal analysis of an EU trading scheme for maritime emissions</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S096585641500107X?via%3Dihub</t>
+  </si>
+  <si>
+    <t>- Arguest that including maritime shipping creates a dilemma. 
+- From an economic point of view the emissions from the entire voyage should be taxed.  
+- From a legal point of view this would likely violate international law</t>
+  </si>
+  <si>
+    <t>Koesler et.al 2015</t>
+  </si>
+  <si>
+    <t>Course set for a cap? A case study among ship operators on a maritime ETS</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0967070X1400208X?via%3Dihub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Investigate the organisational and operational implications of an ETS. 
+- They see no reason why it would not work in practise. 
+- Maritime ETS can engage in cost efficient reductions of carbon emissions. 
+- Monitoring, reporting and trading costs are likely low. 
+- Price volatility and limited supply could be a problem. </t>
+  </si>
+  <si>
+    <t>Franc and Sutto 2013</t>
+  </si>
+  <si>
+    <t>Impact analysis on shipping lines and European ports of a cap- and-trade system on CO2 emissions in maritime transport</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/abs/10.1080/03088839.2013.782440</t>
+  </si>
+  <si>
+    <t>- Studied the implications of an cap and trade system om liner shipping and ports in EU.</t>
+  </si>
+  <si>
+    <t>Wang et.al 2015</t>
+  </si>
+  <si>
+    <t>Modeling the impacts of alternative emission trading schemes on international shipping</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0965856415000841?via%3Dihub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Compare open ETS to a Martitime only ETS (METS). 
+- Either scheme wil lead to lower speed, carrier output and fuel consumption. 
+- Under open ETS dry bulk wil suffer from higher proportional reduction in output and wil sell more permits/buy fewer. 
+- Under METS container shippers wil purchase permits from dry bulk. 
+- Under METS there wil be spillover effects, when the sector that sell is more collusive then the permit price wil rise. </t>
+  </si>
+  <si>
+    <t>Psaraftis 2016</t>
+  </si>
+  <si>
+    <t>Green Maritime Logistics: The Quest for Win-win Solutions</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S2352146516300497?via%3Dihub</t>
+  </si>
+  <si>
+    <t>- Provide an overview of challenges of green maritime logistics and provide examples of emissions (??)</t>
+  </si>
+  <si>
+    <t>Meng et.al 2023</t>
+  </si>
+  <si>
+    <t>Information spillovers between carbon emissions trading prices and shipping markets: A time-frequency analysis</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0140988323001020?via%3Dihub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Use wavelete analysis and spillover index methods to explore the dynamic dependence and information spillovers between the carbon finance market and shipping.
+- Long term dependence and information linkage between carbon finance markets and shipping markets. 
+- Strongest dependence between EU carbon markets and dry bulk shipping. </t>
+  </si>
+  <si>
+    <t>Fuel transition</t>
+  </si>
+  <si>
+    <t>Solakivi 2022</t>
+  </si>
+  <si>
+    <t>Cost competitiveness of alternative maritime fuels in the new regulatory framework</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1361920922003261</t>
+  </si>
+  <si>
+    <t>- Can use this as a basis for the fuel cost model 
+- Investigates when low - and no-emission fuels wil become cost compettative. 
+- Models cost impact on individual vessels 
+- Find that prices wil remain high</t>
+  </si>
+  <si>
+    <t>Is There Business Potential for Sustainable Shipping? Price Premiums Needed to Cover Decarbonized Transportation</t>
+  </si>
+  <si>
+    <t>Schwartz et al 2022</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2071-1050/14/10/5888</t>
+  </si>
+  <si>
+    <t>- Estimates the price premium requiered to ship gods with alternative fuels.
+-Adopting alternative fuels wil lead to a small increase in price</t>
+  </si>
+  <si>
+    <t>Renewable methanol as a fuel for the shipping industry</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S1364032118304945?via%3Dihub</t>
+  </si>
+  <si>
+    <t>-Literature review of the opportunities for methanole in shipping
+-Technicaly viable, and a supply chain exist. 
+- Minor economic barriers exist</t>
+  </si>
+  <si>
+    <t>The Adoption of Liquefied Natural Gas as a Ship Fuel: A Systematic Review of Perspectives and Challenges</t>
+  </si>
+  <si>
+    <t>Wang and Notteboom 2014</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>- Literature review of LNG in shipping</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1080/01441647.2014.981884</t>
+  </si>
+  <si>
+    <t>How can LNG-fuelled ships meet decarbonisation targets? An environmental and economic analysis</t>
+  </si>
+  <si>
+    <t>Svanberg et al2018</t>
+  </si>
+  <si>
+    <t>Balcombe</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0360544221007118?via%3Dihub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Enviormental life cycle and cost analysis of LNG as a shipping fuel. 
+- LNG improves air quality, reduce fuel cost, reduce emissions. 
+- Leakage of methane during the supply chain. </t>
+  </si>
+  <si>
+    <t>Balcombe et al., 2019</t>
+  </si>
+  <si>
+    <t>Balcombe et al., 2021</t>
+  </si>
+  <si>
+    <t>Deniz &amp; Zincir, 2016</t>
+  </si>
+  <si>
+    <t>Prussi et al., 2021</t>
+  </si>
+  <si>
+    <t>Tan et al., 2022</t>
+  </si>
+  <si>
+    <t>Lindstad et al., 2021</t>
+  </si>
+  <si>
+    <t>How to decarbonise international shipping: Options for fuels, technologies and policies</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0196890418314250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Seminal paper
+- Studies emissions reduction in a policy, tech and enviormental perspective
+- LNG is becoming mainstream, cost reduction, but has a high methane leakage in the supply chain. 
+- Biofuels, hydrogen, nuclear and CCS can reduce further but face greater challanges. 
+- Operational efficiency (slow steaming), ship design and using renewable resources could lead to significant GHG and cost savings. 
+- Need for short term and long term solutions. 
+- LNG could be a short term solution. 
+- Long term solutions require strong insentives. </t>
+  </si>
+  <si>
+    <t>Environmental and economical assessment of alternative marine fuels</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0959652615018119</t>
+  </si>
+  <si>
+    <t>- Comparison of methanol, ethanol, liquefied natural gas and hydrogen.
+- Methanol and ethanol are not suitable alternative fuel for ships.
+- Liquefied natural gas is found as the most suitable alternative fuel for ships.
+- Hydrogen can be the ship fuel in the future after more studies will be done.</t>
+  </si>
+  <si>
+    <t>Potential and limiting factors in the use of alternative fuels in the {European} maritime sector</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S095965262100069X</t>
+  </si>
+  <si>
+    <t>- Analyse the challanges and oppertunities for alternative fuels in Europe
+- Cost and GHG savings are fundemental enablers
+- technical maturity, safety and expertise are also needed. 
+- Demand needs to be supported by infrastructure</t>
+  </si>
+  <si>
+    <t>Reduction of maritime GHG emissions and the potential role of E-fuels</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1361920921003722</t>
+  </si>
+  <si>
+    <t>Lindstad et al., 2020</t>
+  </si>
+  <si>
+    <t>Decarbonizing Maritime Transport: The Importance of Engine Technology and Regulations for LNG to Serve as a Transition Fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Alternative fuels are promising for reducing emissions. 
+- The most robust path to decarbonization is e-fuels via dual-fuel engines. 
+- E-fuels demand significantly higher energy than traditional fuels. 
+- A narrow maritime focus can be conter-productive on a global scale. </t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2071-1050/12/21/8793</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Studies under which conditions LNG can be a transitory fuel. 
+- First, the importance of applying appropriate engine technologies to maximize GHG reductions; 
+- Second, that applying best engine technologies is not economically profitable; 
+- Third, how regulations could be amended to reward best engine technologies.
+- Dual fuel engines can be modified for a modest price to switch to ammonia. </t>
+  </si>
+  <si>
+    <t>Alternative fuel options for low carbon maritime transportation: Pathways to 2050</t>
+  </si>
+  <si>
+    <t>Xing et.al 2021</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0959652621008714?casa_token=sDv8RMHiSA8AAAAA:zB7OB2ptbtysO6TiRSO-cgkM136CyxYvfKoXJ3twUno8GFtIONNzDyjm3tx37XFDPZRA-ZHqG1Q</t>
+  </si>
+  <si>
+    <t>- Important to cite
+-Analyze different paths to low carbon maritime transport</t>
+  </si>
+  <si>
+    <t>Reviewing two decades of cleaner alternative marine fuels: Towards IMO's decarbonization of the maritime transport sector</t>
+  </si>
+  <si>
+    <t>Ampath 2021</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0959652621030675?casa_token=Vi1O2vsd8ZwAAAAA:zGotnw-bMeFssBGs-xd_NaxTK_E2jCjfd3oxwbgZY-vtkvcyAeVwaClytYHL2pyfZZtWcI37WZs#sec2</t>
+  </si>
+  <si>
+    <t>- Have a great table of identified barriers</t>
+  </si>
+  <si>
+    <t>Herdzik 2021</t>
+  </si>
+  <si>
+    <t>Decarbonization of Marine Fuels—The Future of Shipping</t>
+  </si>
+  <si>
+    <t>- Har tabell med utslepp per kg fuel</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/353335037_Decarbonization_of_Marine_Fuels-The_Future_of_Shipping</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -664,6 +975,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -686,7 +1003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -695,6 +1012,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkopling" xfId="1" builtinId="8"/>
@@ -1030,16 +1351,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC862F2E-C0DB-45FF-8712-4389B727DC9A}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="B74" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="38.28515625" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
@@ -1712,7 +2033,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="5" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1782,6 +2103,373 @@
       </c>
       <c r="E53" s="1" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>179</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" t="s">
+        <v>186</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>187</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>204</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>208</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>213</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>218</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="270" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B72" t="s">
+        <v>246</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -1795,6 +2483,7 @@
     <hyperlink ref="E30" r:id="rId7" xr:uid="{BD83DFCB-C003-4942-8B45-C7381D40E6E9}"/>
     <hyperlink ref="E33" r:id="rId8" xr:uid="{E04E90D5-5D4C-41F6-85C0-254FD940E5D7}"/>
     <hyperlink ref="E35" r:id="rId9" xr:uid="{FCCFC530-BA3A-4321-B247-193483F4D61A}"/>
+    <hyperlink ref="B60" r:id="rId10" location="aep-article-footnote-id3" display="https://www.sciencedirect.com/science/article/pii/S2352146516300497?via%3Dihub - aep-article-footnote-id3" xr:uid="{0586419C-0F95-4B71-A899-D137A3A5EE0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>